<commit_message>
Add results for OCR
</commit_message>
<xml_diff>
--- a/benchmark/benchmark_results.xlsx
+++ b/benchmark/benchmark_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phi\GitHub Repos\lmm_benchmark\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9F3776-E98B-4B87-98DB-48CFAE3A73E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E070D30F-7346-4C7E-A694-C66E22D6F813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{CD73F02B-09C9-416D-B18F-5543EEA858BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CD73F02B-09C9-416D-B18F-5543EEA858BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Counting" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Counting!$E$18:$H$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OCR!$E$12:$M$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OCR!$E$22:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="102">
   <si>
     <t>Task</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>['Unknown', 'Sign', 'Chinese characters', '大润发', 'Chinese characters', 'hair care', '中国工商银行', '中国', 'Store', "I'm sorry, but I cannot provide an answer to this question as the image is not clear enough to read the text.", "I'm sorry, but I cannot provide an answer to your question as the image is not clear enough for me to accurately identify the Chinese characters.", 'Sign', 'Chinese characters', 'The Chinese characters in the image are "脑筋急转弯" which translates to "brain teaser" or "riddle" in English.', 'Restaurant', 'Chinese characters', 'Chinese characters', 'not possible', '大润发', 'Chinese characters', 'not possible', 'Sign', 'Restaurant', 'Chinese characters', '大润发', 'The Chinese characters in the image are "中国" which means "China" in English.', "I'm sorry, but I cannot provide an answer to this question as the image is not clear enough to read the text.", 'park', 'not possible', 'The Chinese characters in the image are "足球" which means "soccer" in English.', 'The Chinese characters in the image are "肉" which means "meat."', 'The Chinese characters in the image are "光明磊落" (gēng gōng lěi luò), which can be translated to "bright and honest" or "brilliant and upright."', 'green', 'International', 'Chinese characters', 'Restaurant', 'Sign', 'None', 'Police Station', 'Chinese characters', 'Sign', '大润发', 'Chinese characters', '13887223677', '面馆', 'The Chinese characters in the image are "福" which means "happiness" or "good fortune."', "I'm sorry, but I cannot provide an answer to this question as the image is not clear enough to accurately identify the characters.", 'Chinese characters', 'Restaurant', 'Chinese characters', 'The Chinese characters in the image are "福" and "寿".', 'Restaurant', 'Bank', '中国俱乐部', 'The Chinese characters in the image are "中国" which means "China" in English.', 'The Chinese characters in the image are "脑筋急转弯" which translates to "brain teaser" or "riddle" in English.', 'Sign', 'The Chinese characters in the image are "中国" which means "China" in English.', 'Restaurant', '大润发', "I'm sorry, but I cannot provide an answer to this question as the image is not clear enough to read the text.", 'not possible', 'Chinese characters', 'The Chinese characters in the image are "中国" which means "China" in English.']</t>
+  </si>
+  <si>
+    <t>['教學指南', '玉林报国老店', '八、亲、诱、酱', '佳安洪', '没有', '美容发养发', '沈大厦', '五保大米直销店', '米乐视窗', '中华人民共和国', '上海联合医疗设备有限公司', '泰安风景', '咨询小茶', '演示子', '张记包子店', '请您点击', '测评', '难以辨认', '知道房产', '映春光生石', '文化中心', '国际', '大诸香店', '中国的味道', '五金建材', '徐汇区', '金銀收藏', '楼市·可逸锦苑', '验证码', '编号', '不识别', '跨国点场', '万达药店', '上海外国大学', '什么', '欣赏', '西安여자院', '蓝天', '派出所', '不行', '小 门 面 框', '问三路亮', '中华人民共和国', '13877236777', '白云达吉味轩', '心动如初', '钱鉴', '数据路信', '中国大学', '红楼中闲画', '常住住', '你的温度你的爱', '横益東', '星乐俱乐部', '星星夜店', '加强续', '为何信', '喜动态', '双皮良斗专业', '胡氏特点手工卷面团', '外卖雨雨信', '不认识', '王稼有根', '害虫采核']</t>
+  </si>
+  <si>
+    <t>[' The Chinese characters in the image are "赵氏" and "氏".', ' The Chinese characters in the image are "走路" and "走路".', ' 己庚, 庚辛, 庚辛, 庚辛.', ' 大清饭店.', ' The Chinese characters in the image are "天" (meaning "sky" or "heaven"), "火" (meaning "fire" or "flame"), and "人" (meaning "person" or "human").', ' Hair Care.', ' 河北银行.', ' 大水城.', ' The Chinese characters in the image are "起" and "西".', ' The Chinese characters in the image are "河北" and "省".', ' The Chinese characters in the image are "LASGENTE" and "FRESA".', ' The Chinese characters in the image are "超超超超超超超超超超超超超超', ' 大家都会.', ' The Chinese characters in the image are "起火火".', ' The Chinese characters in the image are "肉" and "烤".', ' 家庭资本.', ' The Chinese characters in the image are "大清" and "永安".', ' The Chinese characters in the image are: 今天 星期二 星期三 星期四 星期五 星期六 �', ' 大汉饭店.', ' The Chinese characters in the image are "赵" and "赵".', ' 我们都想要看到他们的爱好。', ' The Chinese characters in the image are "智慧" and "知己".', ' The Chinese characters in the image are "饭" (fàn) and "馅" (xiàn).', ' The Chinese characters in the image are "高阳" and "高阳".', ' 大清店.', ' The Chinese characters in the image are "起床" and "着床".', ' The Chinese characters in the image are "起床香港".', ' This is a place in China.', ' 4 5 6 7 8 9', ' The Chinese characters in the image are "一黑一白".', ' The Chinese characters in the image are "香菜肉".', ' The Chinese characters in the image are "起床看风暴".', ' 大汉银行.', ' The Chinese characters in the image are "联系" and "外交".', ' The Chinese characters in the image are "".', ' The Chinese characters in the image are "聚合" and "吃".', ' The Chinese characters in the image are "聚" and "美".', ' 100英里', ' This is Beijing.', ' The Chinese characters in the image are "".', ' The Chinese characters in the image are "河北省长春市".', ' The Chinese characters in the image are "品" and "饮".', ' The Chinese characters in the image are "財神財神財神" and "財神財神財神".', ' 13877236777.', ' 面馆隔壁的店叫美食。', ' The Chinese characters in the image are "起事" and "产品".',' 河北省长春市.', ' 请假期', ' The Chinese characters in the image are "肉焼飯店" and "飯店".', ' The Chinese characters in the image are "起火火爆爆爆爆爆爆爆爆爆爆爆', ' The Chinese characters in the image are "永福" and "福禄".', ' The Chinese characters in the image are "起风" and "风暴".', ' 家香菜.', ' 大清水族大厦.', ' The Chinese characters in the image are "Hong Kong" and "Hong Kong".', ' The Chinese characters in the image are "起床银行".', ' The Chinese characters in the image are "百合" and "芦苇".', ' The Chinese characters in the image are "赵" and "郑".', ' The Chinese characters in the image are "食品饮料".', ' The Chinese characters in the image are "赞赞赞赞赞赞赞赞赞赞赞赞赞赞', ' 南海水精.', ' The Chinese characters in the image are "".', ' The Chinese characters in the image are "起美家康".', ' The Chinese characters in the image are "大家都" and "没有".']</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -535,6 +541,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -875,7 +885,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1942B8-2432-4AF0-9A2D-492D4BB1B644}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1737,7 @@
         <v>90</v>
       </c>
       <c r="H13" s="2">
-        <f>_xlfn.RANK.AVG(F13,$F$13:$F$20)</f>
+        <f t="shared" ref="H13:H20" si="1">_xlfn.RANK.AVG(F13,$F$13:$F$20)</f>
         <v>1</v>
       </c>
       <c r="I13" s="14"/>
@@ -1759,7 +1769,7 @@
         <v>86</v>
       </c>
       <c r="H14" s="2">
-        <f>_xlfn.RANK.AVG(F14,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I14" s="14"/>
@@ -1787,7 +1797,7 @@
         <v>91</v>
       </c>
       <c r="H15" s="2">
-        <f>_xlfn.RANK.AVG(F15,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I15" s="14"/>
@@ -1819,7 +1829,7 @@
         <v>87</v>
       </c>
       <c r="H16" s="2">
-        <f>_xlfn.RANK.AVG(F16,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I16" s="14"/>
@@ -1847,7 +1857,7 @@
         <v>84</v>
       </c>
       <c r="H17" s="2">
-        <f>_xlfn.RANK.AVG(F17,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
       <c r="I17" s="14"/>
@@ -1875,7 +1885,7 @@
         <v>89</v>
       </c>
       <c r="H18" s="2">
-        <f>_xlfn.RANK.AVG(F18,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
       <c r="I18" s="14"/>
@@ -1903,7 +1913,7 @@
         <v>85</v>
       </c>
       <c r="H19" s="2">
-        <f>_xlfn.RANK.AVG(F19,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I19" s="14"/>
@@ -1931,7 +1941,7 @@
         <v>88</v>
       </c>
       <c r="H20" s="2">
-        <f>_xlfn.RANK.AVG(F20,$F$13:$F$20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I20" s="15"/>
@@ -1986,12 +1996,17 @@
       <c r="C23" s="7"/>
       <c r="D23" s="14"/>
       <c r="E23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" s="2">
+        <f>_xlfn.RANK.AVG(F23,$F$23:$F$30)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2000,12 +2015,17 @@
       <c r="C24" s="7"/>
       <c r="D24" s="14"/>
       <c r="E24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="2">
+        <f>_xlfn.RANK.AVG(F24,$F$23:$F$30)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2014,16 +2034,17 @@
       <c r="C25" s="7"/>
       <c r="D25" s="14"/>
       <c r="E25" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>24</v>
+        <v>0.05</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="2">
+        <f>_xlfn.RANK.AVG(F25,$F$23:$F$30)</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2032,16 +2053,17 @@
       <c r="C26" s="7"/>
       <c r="D26" s="14"/>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F26" s="2">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="H26" s="2">
+        <f>_xlfn.RANK.AVG(F26,$F$23:$F$30)</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2050,16 +2072,17 @@
       <c r="C27" s="7"/>
       <c r="D27" s="14"/>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F27" s="2">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>24</v>
+        <v>97</v>
+      </c>
+      <c r="H27" s="2">
+        <f>_xlfn.RANK.AVG(F27,$F$23:$F$30)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2068,16 +2091,17 @@
       <c r="C28" s="7"/>
       <c r="D28" s="14"/>
       <c r="E28" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>24</v>
+        <v>101</v>
+      </c>
+      <c r="H28" s="2">
+        <f>_xlfn.RANK.AVG(F28,$F$23:$F$30)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2086,16 +2110,17 @@
       <c r="C29" s="7"/>
       <c r="D29" s="14"/>
       <c r="E29" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F29" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="2">
+        <f>_xlfn.RANK.AVG(F29,$F$23:$F$30)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2104,40 +2129,41 @@
       <c r="C30" s="8"/>
       <c r="D30" s="15"/>
       <c r="E30" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F30" s="2">
-        <v>0.78</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>24</v>
+        <v>98</v>
+      </c>
+      <c r="H30" s="2">
+        <f>_xlfn.RANK.AVG(F30,$F$23:$F$30)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E12:M20" xr:uid="{FE1942B8-2432-4AF0-9A2D-492D4BB1B644}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E13:M20">
-      <sortCondition ref="H12:H20"/>
+  <autoFilter ref="E22:H30" xr:uid="{FE1942B8-2432-4AF0-9A2D-492D4BB1B644}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E23:H30">
+      <sortCondition ref="H22:H30"/>
     </sortState>
   </autoFilter>
   <mergeCells count="15">
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="I12:I20"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D2:D10"/>
     <mergeCell ref="C12:C20"/>
     <mergeCell ref="D12:D20"/>
-    <mergeCell ref="A12:A20"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:B30"/>
-    <mergeCell ref="C22:C30"/>
-    <mergeCell ref="D22:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{587588C2-8ED3-412A-B3A3-1899E3119A6C}"/>
@@ -2152,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A52367-4350-4D41-A125-1C847EF2D7DF}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,11 +2621,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="A11:H11"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="B22:B30"/>
@@ -2609,6 +2630,11 @@
     <mergeCell ref="B12:B20"/>
     <mergeCell ref="C12:C20"/>
     <mergeCell ref="D12:D20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="A11:H11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" xr:uid="{2D62BC00-3BFC-42B6-8D8C-52CFB5908C4A}"/>

</xml_diff>